<commit_message>
Modify the output && update the record
</commit_message>
<xml_diff>
--- a/LLMParticipant-Milgram.xlsx
+++ b/LLMParticipant-Milgram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasb/Library/Mobile Documents/com~apple~CloudDocs/Documents/develop/LLMParticipant-Milgram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2A67F4-D337-0F4F-AA60-33DFF8CDA54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D62548-CF4E-E54C-BD71-65789B9E9734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{1C5753A2-A0AA-D14F-8F9E-4DD0EC79A1CE}"/>
+    <workbookView minimized="1" xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{1C5753A2-A0AA-D14F-8F9E-4DD0EC79A1CE}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationTrial" sheetId="1" r:id="rId1"/>
@@ -2709,7 +2709,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix indentation in awareness_probe_prompt English prompt
Corrected the indentation of the English prompt string in the awareness_probe_prompt function for better readability and consistency.
</commit_message>
<xml_diff>
--- a/LLMParticipant-Milgram.xlsx
+++ b/LLMParticipant-Milgram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasb/Library/Mobile Documents/com~apple~CloudDocs/Documents/develop/LLMParticipant-Milgram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D62548-CF4E-E54C-BD71-65789B9E9734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98DFC60-482D-0849-83CC-0B4C6644DC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{1C5753A2-A0AA-D14F-8F9E-4DD0EC79A1CE}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{1C5753A2-A0AA-D14F-8F9E-4DD0EC79A1CE}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidationTrial" sheetId="1" r:id="rId1"/>
@@ -419,6 +419,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-DF24-CB4B-9804-E0E7A969F6ED}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -435,6 +440,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-DF24-CB4B-9804-E0E7A969F6ED}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -451,6 +461,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-DF24-CB4B-9804-E0E7A969F6ED}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -467,6 +482,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-DF24-CB4B-9804-E0E7A969F6ED}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2390,9 +2410,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2430,7 +2450,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2536,7 +2556,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2678,7 +2698,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2709,7 +2729,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>